<commit_message>
updated user stories and backlog, added sprint goal
</commit_message>
<xml_diff>
--- a/Backlog Revised.xlsx
+++ b/Backlog Revised.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anumi\Documents\Sprint 1 - Spec\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anumi\Documents\Sprint 1 - Spec\spec_game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EFA00D-31DD-46EF-94DB-5B8A6AEC6036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE661EAC-D7B7-4439-B11E-D03BBE494416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Backlog Item</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>Task: Handle conditions to award bonus when the last card is revealed</t>
+  </si>
+  <si>
+    <t>User story: Preventing Duplicate Joker Calls</t>
+  </si>
+  <si>
+    <t>Task: Implement feature to prevent a player from calling Joker if all Joker cards are revealed</t>
   </si>
 </sst>
 </file>
@@ -449,15 +455,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4623274-B69E-4769-9C6C-23DA31716F87}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="66.5546875" customWidth="1"/>
+    <col min="1" max="1" width="77" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="26.109375" customWidth="1"/>
   </cols>
@@ -678,6 +684,24 @@
       </c>
       <c r="C23" s="3"/>
     </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="2">
+        <v>3</v>
+      </c>
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="3">
+        <v>3</v>
+      </c>
+      <c r="C25" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>